<commit_message>
fix: solved day 1 part 1
</commit_message>
<xml_diff>
--- a/2022/01_rock_paper_scissors/check.xlsx
+++ b/2022/01_rock_paper_scissors/check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruslanbergenov/Documents/advent_of_code/2022/01_rock_paper_scissors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A55725-9394-4748-A4D4-66E3474FE3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4A2A31-10AB-C14A-AB1A-9656DD99793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="20140" activeTab="1" xr2:uid="{18FE7C4D-A6C7-0445-804D-8EF1DFF06103}"/>
+    <workbookView xWindow="66060" yWindow="9000" windowWidth="25600" windowHeight="20140" activeTab="1" xr2:uid="{18FE7C4D-A6C7-0445-804D-8EF1DFF06103}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$F$2501</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -510,7 +510,7 @@
   <dimension ref="A1:M2501"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="I2" sqref="I2:I2501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -577,12 +577,12 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <f>E2+G2*6+H2*E2</f>
+        <f>E2+G2*6+H2*3</f>
         <v>2</v>
       </c>
       <c r="K2">
         <f>SUM(I:I)</f>
-        <v>12992</v>
+        <v>13268</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -618,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I66" si="7">E3+G3*6+H3*E3</f>
+        <f t="shared" ref="I3:I66" si="7">E3+G3*6+H3*3</f>
         <v>9</v>
       </c>
     </row>
@@ -730,7 +730,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="I25">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="I34">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="I46">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2477,7 +2477,7 @@
       </c>
       <c r="I52">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2958,7 +2958,7 @@
       </c>
       <c r="I65">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -3031,8 +3031,8 @@
         <v>1</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I130" si="15">E67+G67*6+H67*E67</f>
-        <v>2</v>
+        <f t="shared" ref="I67:I130" si="15">E67+G67*6+H67*3</f>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -5399,8 +5399,8 @@
         <v>1</v>
       </c>
       <c r="I131">
-        <f t="shared" ref="I131:I194" si="23">E131+G131*6+H131*E131</f>
-        <v>2</v>
+        <f t="shared" ref="I131:I194" si="23">E131+G131*6+H131*3</f>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -7139,7 +7139,7 @@
       </c>
       <c r="I178">
         <f t="shared" si="23"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="179" spans="1:9">
@@ -7767,7 +7767,7 @@
         <v>0</v>
       </c>
       <c r="I195">
-        <f t="shared" ref="I195:I258" si="31">E195+G195*6+H195*E195</f>
+        <f t="shared" ref="I195:I258" si="31">E195+G195*6+H195*3</f>
         <v>2</v>
       </c>
     </row>
@@ -8508,7 +8508,7 @@
       </c>
       <c r="I215">
         <f t="shared" si="31"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="216" spans="1:9">
@@ -9655,7 +9655,7 @@
       </c>
       <c r="I246">
         <f t="shared" si="31"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="247" spans="1:9">
@@ -10135,7 +10135,7 @@
         <v>0</v>
       </c>
       <c r="I259">
-        <f t="shared" ref="I259:I322" si="39">E259+G259*6+H259*E259</f>
+        <f t="shared" ref="I259:I322" si="39">E259+G259*6+H259*3</f>
         <v>2</v>
       </c>
     </row>
@@ -10247,7 +10247,7 @@
       </c>
       <c r="I262">
         <f t="shared" si="39"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="263" spans="1:9">
@@ -11061,7 +11061,7 @@
       </c>
       <c r="I284">
         <f t="shared" si="39"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="285" spans="1:9">
@@ -11579,7 +11579,7 @@
       </c>
       <c r="I298">
         <f t="shared" si="39"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="299" spans="1:9">
@@ -11986,7 +11986,7 @@
       </c>
       <c r="I309">
         <f t="shared" si="39"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="310" spans="1:9">
@@ -12023,7 +12023,7 @@
       </c>
       <c r="I310">
         <f t="shared" si="39"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="311" spans="1:9">
@@ -12503,7 +12503,7 @@
         <v>1</v>
       </c>
       <c r="I323">
-        <f t="shared" ref="I323:I386" si="47">E323+G323*6+H323*E323</f>
+        <f t="shared" ref="I323:I386" si="47">E323+G323*6+H323*3</f>
         <v>6</v>
       </c>
     </row>
@@ -13170,7 +13170,7 @@
       </c>
       <c r="I341">
         <f t="shared" si="47"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="342" spans="1:9">
@@ -14502,7 +14502,7 @@
       </c>
       <c r="I377">
         <f t="shared" si="47"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="378" spans="1:9">
@@ -14871,7 +14871,7 @@
         <v>1</v>
       </c>
       <c r="I387">
-        <f t="shared" ref="I387:I450" si="55">E387+G387*6+H387*E387</f>
+        <f t="shared" ref="I387:I450" si="55">E387+G387*6+H387*3</f>
         <v>6</v>
       </c>
     </row>
@@ -16167,7 +16167,7 @@
       </c>
       <c r="I422">
         <f t="shared" si="55"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="423" spans="1:9">
@@ -16611,7 +16611,7 @@
       </c>
       <c r="I434">
         <f t="shared" si="55"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="435" spans="1:9">
@@ -17018,7 +17018,7 @@
       </c>
       <c r="I445">
         <f t="shared" si="55"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="446" spans="1:9">
@@ -17239,7 +17239,7 @@
         <v>0</v>
       </c>
       <c r="I451">
-        <f t="shared" ref="I451:I514" si="63">E451+G451*6+H451*E451</f>
+        <f t="shared" ref="I451:I514" si="63">E451+G451*6+H451*3</f>
         <v>2</v>
       </c>
     </row>
@@ -17388,7 +17388,7 @@
       </c>
       <c r="I455">
         <f t="shared" si="63"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="456" spans="1:9">
@@ -18794,7 +18794,7 @@
       </c>
       <c r="I493">
         <f t="shared" si="63"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="494" spans="1:9">
@@ -18831,7 +18831,7 @@
       </c>
       <c r="I494">
         <f t="shared" si="63"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="495" spans="1:9">
@@ -19497,7 +19497,7 @@
       </c>
       <c r="I512">
         <f t="shared" si="63"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="513" spans="1:9">
@@ -19607,7 +19607,7 @@
         <v>0</v>
       </c>
       <c r="I515">
-        <f t="shared" ref="I515:I578" si="71">E515+G515*6+H515*E515</f>
+        <f t="shared" ref="I515:I578" si="71">E515+G515*6+H515*3</f>
         <v>8</v>
       </c>
     </row>
@@ -19719,7 +19719,7 @@
       </c>
       <c r="I518">
         <f t="shared" si="71"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="519" spans="1:9">
@@ -20644,7 +20644,7 @@
       </c>
       <c r="I543">
         <f t="shared" si="71"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="544" spans="1:9">
@@ -20866,7 +20866,7 @@
       </c>
       <c r="I549">
         <f t="shared" si="71"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="550" spans="1:9">
@@ -21051,7 +21051,7 @@
       </c>
       <c r="I554">
         <f t="shared" si="71"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="555" spans="1:9">
@@ -21199,7 +21199,7 @@
       </c>
       <c r="I558">
         <f t="shared" si="71"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="559" spans="1:9">
@@ -21236,7 +21236,7 @@
       </c>
       <c r="I559">
         <f t="shared" si="71"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="560" spans="1:9">
@@ -21421,7 +21421,7 @@
       </c>
       <c r="I564">
         <f t="shared" si="71"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="565" spans="1:9">
@@ -21975,7 +21975,7 @@
         <v>0</v>
       </c>
       <c r="I579">
-        <f t="shared" ref="I579:I642" si="79">E579+G579*6+H579*E579</f>
+        <f t="shared" ref="I579:I642" si="79">E579+G579*6+H579*3</f>
         <v>7</v>
       </c>
     </row>
@@ -22198,7 +22198,7 @@
       </c>
       <c r="I585">
         <f t="shared" si="79"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="586" spans="1:9">
@@ -22827,7 +22827,7 @@
       </c>
       <c r="I602">
         <f t="shared" si="79"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="603" spans="1:9">
@@ -23493,7 +23493,7 @@
       </c>
       <c r="I620">
         <f t="shared" si="79"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="621" spans="1:9">
@@ -23752,7 +23752,7 @@
       </c>
       <c r="I627">
         <f t="shared" si="79"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="628" spans="1:9">
@@ -23826,7 +23826,7 @@
       </c>
       <c r="I629">
         <f t="shared" si="79"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="630" spans="1:9">
@@ -23863,7 +23863,7 @@
       </c>
       <c r="I630">
         <f t="shared" si="79"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="631" spans="1:9">
@@ -24270,7 +24270,7 @@
       </c>
       <c r="I641">
         <f t="shared" si="79"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="642" spans="1:9">
@@ -24343,7 +24343,7 @@
         <v>1</v>
       </c>
       <c r="I643">
-        <f t="shared" ref="I643:I706" si="87">E643+G643*6+H643*E643</f>
+        <f t="shared" ref="I643:I706" si="87">E643+G643*6+H643*3</f>
         <v>6</v>
       </c>
     </row>
@@ -24566,7 +24566,7 @@
       </c>
       <c r="I649">
         <f t="shared" si="87"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="650" spans="1:9">
@@ -24936,7 +24936,7 @@
       </c>
       <c r="I659">
         <f t="shared" si="87"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="660" spans="1:9">
@@ -25565,7 +25565,7 @@
       </c>
       <c r="I676">
         <f t="shared" si="87"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="677" spans="1:9">
@@ -26564,7 +26564,7 @@
       </c>
       <c r="I703">
         <f t="shared" si="87"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="704" spans="1:9">
@@ -26711,7 +26711,7 @@
         <v>0</v>
       </c>
       <c r="I707">
-        <f t="shared" ref="I707:I770" si="95">E707+G707*6+H707*E707</f>
+        <f t="shared" ref="I707:I770" si="95">E707+G707*6+H707*3</f>
         <v>2</v>
       </c>
     </row>
@@ -26749,7 +26749,7 @@
       </c>
       <c r="I708">
         <f t="shared" si="95"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="709" spans="1:9">
@@ -26786,7 +26786,7 @@
       </c>
       <c r="I709">
         <f t="shared" si="95"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="710" spans="1:9">
@@ -27119,7 +27119,7 @@
       </c>
       <c r="I718">
         <f t="shared" si="95"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="719" spans="1:9">
@@ -27415,7 +27415,7 @@
       </c>
       <c r="I726">
         <f t="shared" si="95"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="727" spans="1:9">
@@ -27674,7 +27674,7 @@
       </c>
       <c r="I733">
         <f t="shared" si="95"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="734" spans="1:9">
@@ -27748,7 +27748,7 @@
       </c>
       <c r="I735">
         <f t="shared" si="95"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="736" spans="1:9">
@@ -28377,7 +28377,7 @@
       </c>
       <c r="I752">
         <f t="shared" si="95"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="753" spans="1:9">
@@ -29079,7 +29079,7 @@
         <v>0</v>
       </c>
       <c r="I771">
-        <f t="shared" ref="I771:I834" si="103">E771+G771*6+H771*E771</f>
+        <f t="shared" ref="I771:I834" si="103">E771+G771*6+H771*3</f>
         <v>2</v>
       </c>
     </row>
@@ -29561,7 +29561,7 @@
       </c>
       <c r="I784">
         <f t="shared" si="103"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="785" spans="1:9">
@@ -30338,7 +30338,7 @@
       </c>
       <c r="I805">
         <f t="shared" si="103"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="806" spans="1:9">
@@ -30782,7 +30782,7 @@
       </c>
       <c r="I817">
         <f t="shared" si="103"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="818" spans="1:9">
@@ -31447,7 +31447,7 @@
         <v>0</v>
       </c>
       <c r="I835">
-        <f t="shared" ref="I835:I898" si="111">E835+G835*6+H835*E835</f>
+        <f t="shared" ref="I835:I898" si="111">E835+G835*6+H835*3</f>
         <v>7</v>
       </c>
     </row>
@@ -31559,7 +31559,7 @@
       </c>
       <c r="I838">
         <f t="shared" si="111"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="839" spans="1:9">
@@ -31633,7 +31633,7 @@
       </c>
       <c r="I840">
         <f t="shared" si="111"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="841" spans="1:9">
@@ -31929,7 +31929,7 @@
       </c>
       <c r="I848">
         <f t="shared" si="111"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="849" spans="1:9">
@@ -32743,7 +32743,7 @@
       </c>
       <c r="I870">
         <f t="shared" si="111"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="871" spans="1:9">
@@ -33150,7 +33150,7 @@
       </c>
       <c r="I881">
         <f t="shared" si="111"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="882" spans="1:9">
@@ -33557,7 +33557,7 @@
       </c>
       <c r="I892">
         <f t="shared" si="111"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="893" spans="1:9">
@@ -33815,7 +33815,7 @@
         <v>1</v>
       </c>
       <c r="I899">
-        <f t="shared" ref="I899:I962" si="119">E899+G899*6+H899*E899</f>
+        <f t="shared" ref="I899:I962" si="119">E899+G899*6+H899*3</f>
         <v>6</v>
       </c>
     </row>
@@ -33927,7 +33927,7 @@
       </c>
       <c r="I902">
         <f t="shared" si="119"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="903" spans="1:9">
@@ -34260,7 +34260,7 @@
       </c>
       <c r="I911">
         <f t="shared" si="119"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="912" spans="1:9">
@@ -36183,7 +36183,7 @@
         <v>0</v>
       </c>
       <c r="I963">
-        <f t="shared" ref="I963:I1026" si="127">E963+G963*6+H963*E963</f>
+        <f t="shared" ref="I963:I1026" si="127">E963+G963*6+H963*3</f>
         <v>2</v>
       </c>
     </row>
@@ -36332,7 +36332,7 @@
       </c>
       <c r="I967">
         <f t="shared" si="127"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="968" spans="1:9">
@@ -37442,7 +37442,7 @@
       </c>
       <c r="I997">
         <f t="shared" si="127"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="998" spans="1:9">
@@ -38145,7 +38145,7 @@
       </c>
       <c r="I1016">
         <f t="shared" si="127"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1017" spans="1:9">
@@ -38367,7 +38367,7 @@
       </c>
       <c r="I1022">
         <f t="shared" si="127"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1023" spans="1:9">
@@ -38551,7 +38551,7 @@
         <v>1</v>
       </c>
       <c r="I1027">
-        <f t="shared" ref="I1027:I1090" si="135">E1027+G1027*6+H1027*E1027</f>
+        <f t="shared" ref="I1027:I1090" si="135">E1027+G1027*6+H1027*3</f>
         <v>6</v>
       </c>
     </row>
@@ -39366,7 +39366,7 @@
       </c>
       <c r="I1049">
         <f t="shared" si="135"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1050" spans="1:9">
@@ -39588,7 +39588,7 @@
       </c>
       <c r="I1055">
         <f t="shared" si="135"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1056" spans="1:9">
@@ -40550,7 +40550,7 @@
       </c>
       <c r="I1081">
         <f t="shared" si="135"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1082" spans="1:9">
@@ -40587,7 +40587,7 @@
       </c>
       <c r="I1082">
         <f t="shared" si="135"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1083" spans="1:9">
@@ -40624,7 +40624,7 @@
       </c>
       <c r="I1083">
         <f t="shared" si="135"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1084" spans="1:9">
@@ -40919,7 +40919,7 @@
         <v>0</v>
       </c>
       <c r="I1091">
-        <f t="shared" ref="I1091:I1154" si="143">E1091+G1091*6+H1091*E1091</f>
+        <f t="shared" ref="I1091:I1154" si="143">E1091+G1091*6+H1091*3</f>
         <v>9</v>
       </c>
     </row>
@@ -41697,7 +41697,7 @@
       </c>
       <c r="I1112">
         <f t="shared" si="143"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1113" spans="1:9">
@@ -42622,7 +42622,7 @@
       </c>
       <c r="I1137">
         <f t="shared" si="143"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1138" spans="1:9">
@@ -42659,7 +42659,7 @@
       </c>
       <c r="I1138">
         <f t="shared" si="143"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1139" spans="1:9">
@@ -42992,7 +42992,7 @@
       </c>
       <c r="I1147">
         <f t="shared" si="143"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1148" spans="1:9">
@@ -43287,7 +43287,7 @@
         <v>0</v>
       </c>
       <c r="I1155">
-        <f t="shared" ref="I1155:I1218" si="151">E1155+G1155*6+H1155*E1155</f>
+        <f t="shared" ref="I1155:I1218" si="151">E1155+G1155*6+H1155*3</f>
         <v>2</v>
       </c>
     </row>
@@ -43436,7 +43436,7 @@
       </c>
       <c r="I1159">
         <f t="shared" si="151"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1160" spans="1:9">
@@ -44250,7 +44250,7 @@
       </c>
       <c r="I1181">
         <f t="shared" si="151"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1182" spans="1:9">
@@ -44287,7 +44287,7 @@
       </c>
       <c r="I1182">
         <f t="shared" si="151"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1183" spans="1:9">
@@ -44361,7 +44361,7 @@
       </c>
       <c r="I1184">
         <f t="shared" si="151"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1185" spans="1:9">
@@ -45027,7 +45027,7 @@
       </c>
       <c r="I1202">
         <f t="shared" si="151"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1203" spans="1:9">
@@ -45360,7 +45360,7 @@
       </c>
       <c r="I1211">
         <f t="shared" si="151"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1212" spans="1:9">
@@ -45582,7 +45582,7 @@
       </c>
       <c r="I1217">
         <f t="shared" si="151"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1218" spans="1:9">
@@ -45655,7 +45655,7 @@
         <v>0</v>
       </c>
       <c r="I1219">
-        <f t="shared" ref="I1219:I1282" si="159">E1219+G1219*6+H1219*E1219</f>
+        <f t="shared" ref="I1219:I1282" si="159">E1219+G1219*6+H1219*3</f>
         <v>9</v>
       </c>
     </row>
@@ -46581,7 +46581,7 @@
       </c>
       <c r="I1244">
         <f t="shared" si="159"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1245" spans="1:9">
@@ -47580,7 +47580,7 @@
       </c>
       <c r="I1271">
         <f t="shared" si="159"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1272" spans="1:9">
@@ -48023,7 +48023,7 @@
         <v>1</v>
       </c>
       <c r="I1283">
-        <f t="shared" ref="I1283:I1346" si="167">E1283+G1283*6+H1283*E1283</f>
+        <f t="shared" ref="I1283:I1346" si="167">E1283+G1283*6+H1283*3</f>
         <v>6</v>
       </c>
     </row>
@@ -49763,7 +49763,7 @@
       </c>
       <c r="I1330">
         <f t="shared" si="167"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1331" spans="1:9">
@@ -50244,7 +50244,7 @@
       </c>
       <c r="I1343">
         <f t="shared" si="167"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1344" spans="1:9">
@@ -50391,7 +50391,7 @@
         <v>0</v>
       </c>
       <c r="I1347">
-        <f t="shared" ref="I1347:I1410" si="175">E1347+G1347*6+H1347*E1347</f>
+        <f t="shared" ref="I1347:I1410" si="175">E1347+G1347*6+H1347*3</f>
         <v>2</v>
       </c>
     </row>
@@ -51132,7 +51132,7 @@
       </c>
       <c r="I1367">
         <f t="shared" si="175"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1368" spans="1:9">
@@ -51391,7 +51391,7 @@
       </c>
       <c r="I1374">
         <f t="shared" si="175"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1375" spans="1:9">
@@ -51465,7 +51465,7 @@
       </c>
       <c r="I1376">
         <f t="shared" si="175"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1377" spans="1:9">
@@ -51502,7 +51502,7 @@
       </c>
       <c r="I1377">
         <f t="shared" si="175"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1378" spans="1:9">
@@ -51539,7 +51539,7 @@
       </c>
       <c r="I1378">
         <f t="shared" si="175"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1379" spans="1:9">
@@ -52316,7 +52316,7 @@
       </c>
       <c r="I1399">
         <f t="shared" si="175"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1400" spans="1:9">
@@ -52759,7 +52759,7 @@
         <v>0</v>
       </c>
       <c r="I1411">
-        <f t="shared" ref="I1411:I1474" si="183">E1411+G1411*6+H1411*E1411</f>
+        <f t="shared" ref="I1411:I1474" si="183">E1411+G1411*6+H1411*3</f>
         <v>9</v>
       </c>
     </row>
@@ -53463,7 +53463,7 @@
       </c>
       <c r="I1430">
         <f t="shared" si="183"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1431" spans="1:9">
@@ -54203,7 +54203,7 @@
       </c>
       <c r="I1450">
         <f t="shared" si="183"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1451" spans="1:9">
@@ -54721,7 +54721,7 @@
       </c>
       <c r="I1464">
         <f t="shared" si="183"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1465" spans="1:9">
@@ -54906,7 +54906,7 @@
       </c>
       <c r="I1469">
         <f t="shared" si="183"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1470" spans="1:9">
@@ -55017,7 +55017,7 @@
       </c>
       <c r="I1472">
         <f t="shared" si="183"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1473" spans="1:9">
@@ -55127,7 +55127,7 @@
         <v>0</v>
       </c>
       <c r="I1475">
-        <f t="shared" ref="I1475:I1538" si="191">E1475+G1475*6+H1475*E1475</f>
+        <f t="shared" ref="I1475:I1538" si="191">E1475+G1475*6+H1475*3</f>
         <v>9</v>
       </c>
     </row>
@@ -55905,7 +55905,7 @@
       </c>
       <c r="I1496">
         <f t="shared" si="191"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1497" spans="1:9">
@@ -56645,7 +56645,7 @@
       </c>
       <c r="I1516">
         <f t="shared" si="191"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1517" spans="1:9">
@@ -57052,7 +57052,7 @@
       </c>
       <c r="I1527">
         <f t="shared" si="191"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1528" spans="1:9">
@@ -57385,7 +57385,7 @@
       </c>
       <c r="I1536">
         <f t="shared" si="191"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1537" spans="1:9">
@@ -57495,7 +57495,7 @@
         <v>1</v>
       </c>
       <c r="I1539">
-        <f t="shared" ref="I1539:I1602" si="199">E1539+G1539*6+H1539*E1539</f>
+        <f t="shared" ref="I1539:I1602" si="199">E1539+G1539*6+H1539*3</f>
         <v>6</v>
       </c>
     </row>
@@ -58717,7 +58717,7 @@
       </c>
       <c r="I1572">
         <f t="shared" si="199"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1573" spans="1:9">
@@ -59827,7 +59827,7 @@
       </c>
       <c r="I1602">
         <f t="shared" si="199"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1603" spans="1:9">
@@ -59863,7 +59863,7 @@
         <v>0</v>
       </c>
       <c r="I1603">
-        <f t="shared" ref="I1603:I1666" si="207">E1603+G1603*6+H1603*E1603</f>
+        <f t="shared" ref="I1603:I1666" si="207">E1603+G1603*6+H1603*3</f>
         <v>2</v>
       </c>
     </row>
@@ -60567,7 +60567,7 @@
       </c>
       <c r="I1622">
         <f t="shared" si="207"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1623" spans="1:9">
@@ -60604,7 +60604,7 @@
       </c>
       <c r="I1623">
         <f t="shared" si="207"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1624" spans="1:9">
@@ -60826,7 +60826,7 @@
       </c>
       <c r="I1629">
         <f t="shared" si="207"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1630" spans="1:9">
@@ -60974,7 +60974,7 @@
       </c>
       <c r="I1633">
         <f t="shared" si="207"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1634" spans="1:9">
@@ -61122,7 +61122,7 @@
       </c>
       <c r="I1637">
         <f t="shared" si="207"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1638" spans="1:9">
@@ -61529,7 +61529,7 @@
       </c>
       <c r="I1648">
         <f t="shared" si="207"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1649" spans="1:9">
@@ -62231,7 +62231,7 @@
         <v>1</v>
       </c>
       <c r="I1667">
-        <f t="shared" ref="I1667:I1730" si="215">E1667+G1667*6+H1667*E1667</f>
+        <f t="shared" ref="I1667:I1730" si="215">E1667+G1667*6+H1667*3</f>
         <v>6</v>
       </c>
     </row>
@@ -62676,7 +62676,7 @@
       </c>
       <c r="I1679">
         <f t="shared" si="215"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1680" spans="1:9">
@@ -62861,7 +62861,7 @@
       </c>
       <c r="I1684">
         <f t="shared" si="215"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1685" spans="1:9">
@@ -62972,7 +62972,7 @@
       </c>
       <c r="I1687">
         <f t="shared" si="215"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1688" spans="1:9">
@@ -64119,7 +64119,7 @@
       </c>
       <c r="I1718">
         <f t="shared" si="215"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1719" spans="1:9">
@@ -64599,7 +64599,7 @@
         <v>0</v>
       </c>
       <c r="I1731">
-        <f t="shared" ref="I1731:I1794" si="223">E1731+G1731*6+H1731*E1731</f>
+        <f t="shared" ref="I1731:I1794" si="223">E1731+G1731*6+H1731*3</f>
         <v>8</v>
       </c>
     </row>
@@ -65118,7 +65118,7 @@
       </c>
       <c r="I1745">
         <f t="shared" si="223"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1746" spans="1:9">
@@ -65155,7 +65155,7 @@
       </c>
       <c r="I1746">
         <f t="shared" si="223"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1747" spans="1:9">
@@ -65673,7 +65673,7 @@
       </c>
       <c r="I1760">
         <f t="shared" si="223"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1761" spans="1:9">
@@ -65710,7 +65710,7 @@
       </c>
       <c r="I1761">
         <f t="shared" si="223"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1762" spans="1:9">
@@ -65969,7 +65969,7 @@
       </c>
       <c r="I1768">
         <f t="shared" si="223"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1769" spans="1:9">
@@ -66154,7 +66154,7 @@
       </c>
       <c r="I1773">
         <f t="shared" si="223"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1774" spans="1:9">
@@ -66967,7 +66967,7 @@
         <v>0</v>
       </c>
       <c r="I1795">
-        <f t="shared" ref="I1795:I1858" si="231">E1795+G1795*6+H1795*E1795</f>
+        <f t="shared" ref="I1795:I1858" si="231">E1795+G1795*6+H1795*3</f>
         <v>9</v>
       </c>
     </row>
@@ -67079,7 +67079,7 @@
       </c>
       <c r="I1798">
         <f t="shared" si="231"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1799" spans="1:9">
@@ -67486,7 +67486,7 @@
       </c>
       <c r="I1809">
         <f t="shared" si="231"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1810" spans="1:9">
@@ -67745,7 +67745,7 @@
       </c>
       <c r="I1816">
         <f t="shared" si="231"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1817" spans="1:9">
@@ -69335,7 +69335,7 @@
         <v>0</v>
       </c>
       <c r="I1859">
-        <f t="shared" ref="I1859:I1922" si="239">E1859+G1859*6+H1859*E1859</f>
+        <f t="shared" ref="I1859:I1922" si="239">E1859+G1859*6+H1859*3</f>
         <v>7</v>
       </c>
     </row>
@@ -70927,7 +70927,7 @@
       </c>
       <c r="I1902">
         <f t="shared" si="239"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1903" spans="1:9">
@@ -71112,7 +71112,7 @@
       </c>
       <c r="I1907">
         <f t="shared" si="239"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1908" spans="1:9">
@@ -71630,7 +71630,7 @@
       </c>
       <c r="I1921">
         <f t="shared" si="239"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1922" spans="1:9">
@@ -71703,7 +71703,7 @@
         <v>1</v>
       </c>
       <c r="I1923">
-        <f t="shared" ref="I1923:I1986" si="247">E1923+G1923*6+H1923*E1923</f>
+        <f t="shared" ref="I1923:I1986" si="247">E1923+G1923*6+H1923*3</f>
         <v>6</v>
       </c>
     </row>
@@ -72185,7 +72185,7 @@
       </c>
       <c r="I1936">
         <f t="shared" si="247"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1937" spans="1:9">
@@ -73110,7 +73110,7 @@
       </c>
       <c r="I1961">
         <f t="shared" si="247"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1962" spans="1:9">
@@ -74071,7 +74071,7 @@
         <v>0</v>
       </c>
       <c r="I1987">
-        <f t="shared" ref="I1987:I2050" si="255">E1987+G1987*6+H1987*E1987</f>
+        <f t="shared" ref="I1987:I2050" si="255">E1987+G1987*6+H1987*3</f>
         <v>9</v>
       </c>
     </row>
@@ -74775,7 +74775,7 @@
       </c>
       <c r="I2006">
         <f t="shared" si="255"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2007" spans="1:9">
@@ -74960,7 +74960,7 @@
       </c>
       <c r="I2011">
         <f t="shared" si="255"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2012" spans="1:9">
@@ -75293,7 +75293,7 @@
       </c>
       <c r="I2020">
         <f t="shared" si="255"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2021" spans="1:9">
@@ -75663,7 +75663,7 @@
       </c>
       <c r="I2030">
         <f t="shared" si="255"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2031" spans="1:9">
@@ -76439,7 +76439,7 @@
         <v>0</v>
       </c>
       <c r="I2051">
-        <f t="shared" ref="I2051:I2114" si="263">E2051+G2051*6+H2051*E2051</f>
+        <f t="shared" ref="I2051:I2114" si="263">E2051+G2051*6+H2051*3</f>
         <v>9</v>
       </c>
     </row>
@@ -77550,7 +77550,7 @@
       </c>
       <c r="I2081">
         <f t="shared" si="263"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2082" spans="1:9">
@@ -77883,7 +77883,7 @@
       </c>
       <c r="I2090">
         <f t="shared" si="263"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2091" spans="1:9">
@@ -77957,7 +77957,7 @@
       </c>
       <c r="I2092">
         <f t="shared" si="263"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2093" spans="1:9">
@@ -78807,7 +78807,7 @@
         <v>1</v>
       </c>
       <c r="I2115">
-        <f t="shared" ref="I2115:I2178" si="271">E2115+G2115*6+H2115*E2115</f>
+        <f t="shared" ref="I2115:I2178" si="271">E2115+G2115*6+H2115*3</f>
         <v>6</v>
       </c>
     </row>
@@ -78993,7 +78993,7 @@
       </c>
       <c r="I2120">
         <f t="shared" si="271"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2121" spans="1:9">
@@ -79067,7 +79067,7 @@
       </c>
       <c r="I2122">
         <f t="shared" si="271"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2123" spans="1:9">
@@ -80214,7 +80214,7 @@
       </c>
       <c r="I2153">
         <f t="shared" si="271"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2154" spans="1:9">
@@ -81175,7 +81175,7 @@
         <v>0</v>
       </c>
       <c r="I2179">
-        <f t="shared" ref="I2179:I2242" si="279">E2179+G2179*6+H2179*E2179</f>
+        <f t="shared" ref="I2179:I2242" si="279">E2179+G2179*6+H2179*3</f>
         <v>3</v>
       </c>
     </row>
@@ -81509,7 +81509,7 @@
       </c>
       <c r="I2188">
         <f t="shared" si="279"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2189" spans="1:9">
@@ -81768,7 +81768,7 @@
       </c>
       <c r="I2195">
         <f t="shared" si="279"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2196" spans="1:9">
@@ -81916,7 +81916,7 @@
       </c>
       <c r="I2199">
         <f t="shared" si="279"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2200" spans="1:9">
@@ -82138,7 +82138,7 @@
       </c>
       <c r="I2205">
         <f t="shared" si="279"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2206" spans="1:9">
@@ -82360,7 +82360,7 @@
       </c>
       <c r="I2211">
         <f t="shared" si="279"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2212" spans="1:9">
@@ -82767,7 +82767,7 @@
       </c>
       <c r="I2222">
         <f t="shared" si="279"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2223" spans="1:9">
@@ -83137,7 +83137,7 @@
       </c>
       <c r="I2232">
         <f t="shared" si="279"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2233" spans="1:9">
@@ -83543,7 +83543,7 @@
         <v>0</v>
       </c>
       <c r="I2243">
-        <f t="shared" ref="I2243:I2306" si="287">E2243+G2243*6+H2243*E2243</f>
+        <f t="shared" ref="I2243:I2306" si="287">E2243+G2243*6+H2243*3</f>
         <v>7</v>
       </c>
     </row>
@@ -84321,7 +84321,7 @@
       </c>
       <c r="I2264">
         <f t="shared" si="287"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2265" spans="1:9">
@@ -84469,7 +84469,7 @@
       </c>
       <c r="I2268">
         <f t="shared" si="287"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2269" spans="1:9">
@@ -84543,7 +84543,7 @@
       </c>
       <c r="I2270">
         <f t="shared" si="287"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2271" spans="1:9">
@@ -84765,7 +84765,7 @@
       </c>
       <c r="I2276">
         <f t="shared" si="287"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2277" spans="1:9">
@@ -85911,7 +85911,7 @@
         <v>0</v>
       </c>
       <c r="I2307">
-        <f t="shared" ref="I2307:I2370" si="295">E2307+G2307*6+H2307*E2307</f>
+        <f t="shared" ref="I2307:I2370" si="295">E2307+G2307*6+H2307*3</f>
         <v>2</v>
       </c>
     </row>
@@ -86060,7 +86060,7 @@
       </c>
       <c r="I2311">
         <f t="shared" si="295"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2312" spans="1:9">
@@ -86171,7 +86171,7 @@
       </c>
       <c r="I2314">
         <f t="shared" si="295"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2315" spans="1:9">
@@ -86208,7 +86208,7 @@
       </c>
       <c r="I2315">
         <f t="shared" si="295"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2316" spans="1:9">
@@ -86578,7 +86578,7 @@
       </c>
       <c r="I2325">
         <f t="shared" si="295"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2326" spans="1:9">
@@ -86911,7 +86911,7 @@
       </c>
       <c r="I2334">
         <f t="shared" si="295"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2335" spans="1:9">
@@ -87466,7 +87466,7 @@
       </c>
       <c r="I2349">
         <f t="shared" si="295"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2350" spans="1:9">
@@ -87725,7 +87725,7 @@
       </c>
       <c r="I2356">
         <f t="shared" si="295"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2357" spans="1:9">
@@ -88279,7 +88279,7 @@
         <v>1</v>
       </c>
       <c r="I2371">
-        <f t="shared" ref="I2371:I2434" si="303">E2371+G2371*6+H2371*E2371</f>
+        <f t="shared" ref="I2371:I2434" si="303">E2371+G2371*6+H2371*3</f>
         <v>6</v>
       </c>
     </row>
@@ -88539,7 +88539,7 @@
       </c>
       <c r="I2378">
         <f t="shared" si="303"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2379" spans="1:9">
@@ -88946,7 +88946,7 @@
       </c>
       <c r="I2389">
         <f t="shared" si="303"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2390" spans="1:9">
@@ -89057,7 +89057,7 @@
       </c>
       <c r="I2392">
         <f t="shared" si="303"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2393" spans="1:9">
@@ -90647,7 +90647,7 @@
         <v>1</v>
       </c>
       <c r="I2435">
-        <f t="shared" ref="I2435:I2498" si="311">E2435+G2435*6+H2435*E2435</f>
+        <f t="shared" ref="I2435:I2498" si="311">E2435+G2435*6+H2435*3</f>
         <v>6</v>
       </c>
     </row>
@@ -90870,7 +90870,7 @@
       </c>
       <c r="I2441">
         <f t="shared" si="311"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2442" spans="1:9">
@@ -91166,7 +91166,7 @@
       </c>
       <c r="I2449">
         <f t="shared" si="311"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2450" spans="1:9">
@@ -91758,7 +91758,7 @@
       </c>
       <c r="I2465">
         <f t="shared" si="311"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2466" spans="1:9">
@@ -92017,7 +92017,7 @@
       </c>
       <c r="I2472">
         <f t="shared" si="311"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2473" spans="1:9">
@@ -93015,7 +93015,7 @@
         <v>0</v>
       </c>
       <c r="I2499">
-        <f t="shared" ref="I2499:I2501" si="319">E2499+G2499*6+H2499*E2499</f>
+        <f t="shared" ref="I2499:I2501" si="319">E2499+G2499*6+H2499*3</f>
         <v>1</v>
       </c>
     </row>
@@ -93053,7 +93053,7 @@
       </c>
       <c r="I2500">
         <f t="shared" si="319"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2501" spans="1:9">

</xml_diff>

<commit_message>
feat: solved day 1 part 2
</commit_message>
<xml_diff>
--- a/2022/01_rock_paper_scissors/check.xlsx
+++ b/2022/01_rock_paper_scissors/check.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruslanbergenov/Documents/advent_of_code/2022/01_rock_paper_scissors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4A2A31-10AB-C14A-AB1A-9656DD99793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD4760C-9EDB-AA4E-8290-276A5E34FA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66060" yWindow="9000" windowWidth="25600" windowHeight="20140" activeTab="1" xr2:uid="{18FE7C4D-A6C7-0445-804D-8EF1DFF06103}"/>
+    <workbookView xWindow="64000" yWindow="1460" windowWidth="25600" windowHeight="20140" xr2:uid="{18FE7C4D-A6C7-0445-804D-8EF1DFF06103}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$F$2501</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1'!$A$1:$I$2501</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2522" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2522" uniqueCount="26">
   <si>
     <t>Y</t>
   </si>
@@ -109,6 +108,15 @@
   </si>
   <si>
     <t>score</t>
+  </si>
+  <si>
+    <t>rock</t>
+  </si>
+  <si>
+    <t>paper</t>
+  </si>
+  <si>
+    <t>scissors</t>
   </si>
 </sst>
 </file>
@@ -466,51 +474,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1330951C-62A8-984D-8F93-F61F9D5AC899}">
-  <dimension ref="E4:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="4" spans="5:6">
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="5:6">
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="5:6">
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82A1DB5-732A-9049-9A4E-38398D2C9222}">
   <dimension ref="A1:M2501"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I2501"/>
+      <selection activeCell="K12" sqref="K12:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -806,6 +774,9 @@
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
       <c r="L8" t="s">
         <v>4</v>
       </c>
@@ -849,6 +820,9 @@
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
       <c r="L9" t="s">
         <v>5</v>
       </c>
@@ -892,6 +866,9 @@
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
       <c r="L10" t="s">
         <v>3</v>
       </c>
@@ -972,6 +949,9 @@
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
+      <c r="K12" t="s">
+        <v>23</v>
+      </c>
       <c r="L12" t="s">
         <v>1</v>
       </c>
@@ -1015,6 +995,9 @@
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
+      <c r="K13" t="s">
+        <v>24</v>
+      </c>
       <c r="L13" t="s">
         <v>0</v>
       </c>
@@ -1057,6 +1040,9 @@
       <c r="I14">
         <f t="shared" si="7"/>
         <v>6</v>
+      </c>
+      <c r="K14" t="s">
+        <v>25</v>
       </c>
       <c r="L14" t="s">
         <v>2</v>

</xml_diff>